<commit_message>
[Docs] image and model samples
</commit_message>
<xml_diff>
--- a/Documents/KeHoachThucHien.xlsx
+++ b/Documents/KeHoachThucHien.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UIT\HK7\Seminar\PROJECT\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C4A41671-53B8-4717-919F-287445B59ECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{745D5224-2078-4309-A583-57745E92A8AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{69850307-C70E-4F0D-824B-1ED21B8CE3E1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="70">
   <si>
     <t>Công việc</t>
   </si>
@@ -95,9 +95,6 @@
     <t>Giai đoạn 1: Nghiên cứu đề tài và chuẩn bị nội dung</t>
   </si>
   <si>
-    <t>Lê Văn Phú - Lê Hoài Hải</t>
-  </si>
-  <si>
     <t>Lê Văn Phú</t>
   </si>
   <si>
@@ -135,9 +132,6 @@
   </si>
   <si>
     <t>2. Thiết kế cơ sở dữ liệu</t>
-  </si>
-  <si>
-    <t>5. Xây dựng backend API</t>
   </si>
   <si>
     <t>Thành phẩm</t>
@@ -174,9 +168,6 @@
     <t>3. Xây dựng giao diện frontend</t>
   </si>
   <si>
-    <t>6. Tích hợp API vào frontend</t>
-  </si>
-  <si>
     <t>Cả hai</t>
   </si>
   <si>
@@ -199,9 +190,6 @@
   </si>
   <si>
     <t>30/11/2024</t>
-  </si>
-  <si>
-    <t>30 ngày</t>
   </si>
   <si>
     <t>Vẽ figma</t>
@@ -234,12 +222,54 @@
   <si>
     <t>Chỉnh sửa những mục còn sót lại</t>
   </si>
+  <si>
+    <t>4. Xây dựng backend API</t>
+    <phoneticPr fontId="0"/>
+  </si>
+  <si>
+    <t>5. Tích hợp API vào frontend</t>
+    <phoneticPr fontId="0"/>
+  </si>
+  <si>
+    <t>20/11/2024</t>
+  </si>
+  <si>
+    <t>Figma</t>
+  </si>
+  <si>
+    <t>ERD</t>
+  </si>
+  <si>
+    <t>repo</t>
+  </si>
+  <si>
+    <t>Document</t>
+  </si>
+  <si>
+    <t>16 ngày</t>
+  </si>
+  <si>
+    <t>10/11/2024</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>10 ngày</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>20 ngày</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>IN PROGRESS</t>
+    <phoneticPr fontId="5"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,6 +293,14 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="游ゴシック"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -325,10 +363,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -402,8 +441,15 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -417,10 +463,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -742,8 +784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91AA6AA8-9363-41C7-9B48-F954A9DD444B}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -779,7 +821,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
@@ -803,7 +845,7 @@
         <v>9</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="4" t="s">
@@ -818,15 +860,17 @@
         <v>11</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="4"/>
+        <v>19</v>
+      </c>
+      <c r="G3" s="26" t="s">
+        <v>64</v>
+      </c>
       <c r="H3" s="4" t="s">
         <v>10</v>
       </c>
@@ -836,18 +880,20 @@
     </row>
     <row r="4" spans="1:9" ht="37.5">
       <c r="A4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>24</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>25</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="4"/>
+        <v>19</v>
+      </c>
+      <c r="G4" s="26" t="s">
+        <v>64</v>
+      </c>
       <c r="H4" s="4" t="s">
         <v>10</v>
       </c>
@@ -857,18 +903,20 @@
     </row>
     <row r="5" spans="1:9" ht="37.5">
       <c r="A5" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="G5" s="26" t="s">
+        <v>64</v>
+      </c>
       <c r="H5" s="4" t="s">
         <v>10</v>
       </c>
@@ -878,18 +926,20 @@
     </row>
     <row r="6" spans="1:9" ht="56.25">
       <c r="A6" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
       <c r="F6" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="4"/>
+        <v>19</v>
+      </c>
+      <c r="G6" s="26" t="s">
+        <v>64</v>
+      </c>
       <c r="H6" s="4" t="s">
         <v>10</v>
       </c>
@@ -899,18 +949,20 @@
     </row>
     <row r="7" spans="1:9" ht="56.25">
       <c r="A7" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
       <c r="F7" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="G7" s="26" t="s">
+        <v>64</v>
+      </c>
       <c r="H7" s="4" t="s">
         <v>10</v>
       </c>
@@ -920,20 +972,20 @@
     </row>
     <row r="8" spans="1:9" ht="49.7" customHeight="1">
       <c r="A8" s="21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" s="11"/>
       <c r="C8" s="12">
         <v>45302</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>16</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="G8" s="13"/>
       <c r="H8" s="14" t="s">
@@ -946,10 +998,10 @@
     </row>
     <row r="9" spans="1:9" ht="20.25">
       <c r="A9" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C9" s="12">
         <v>45302</v>
@@ -958,12 +1010,14 @@
         <v>45362</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F9" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="14"/>
+        <v>19</v>
+      </c>
+      <c r="G9" s="25" t="s">
+        <v>61</v>
+      </c>
       <c r="H9" s="14" t="s">
         <v>10</v>
       </c>
@@ -973,10 +1027,10 @@
     </row>
     <row r="10" spans="1:9" ht="20.25">
       <c r="A10" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C10" s="12">
         <v>45302</v>
@@ -985,12 +1039,14 @@
         <v>45333</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F10" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="G10" s="14"/>
+        <v>20</v>
+      </c>
+      <c r="G10" s="25" t="s">
+        <v>62</v>
+      </c>
       <c r="H10" s="14" t="s">
         <v>10</v>
       </c>
@@ -1000,10 +1056,10 @@
     </row>
     <row r="11" spans="1:9" ht="93.75">
       <c r="A11" s="18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C11" s="12">
         <v>45393</v>
@@ -1012,12 +1068,14 @@
         <v>45607</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F11" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11" s="14"/>
+        <v>19</v>
+      </c>
+      <c r="G11" s="25" t="s">
+        <v>63</v>
+      </c>
       <c r="H11" s="17" t="s">
         <v>10</v>
       </c>
@@ -1027,10 +1085,10 @@
     </row>
     <row r="12" spans="1:9" ht="75">
       <c r="A12" s="18" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C12" s="12">
         <v>45362</v>
@@ -1042,7 +1100,7 @@
         <v>13</v>
       </c>
       <c r="F12" s="24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G12" s="14"/>
       <c r="H12" s="14" t="s">
@@ -1054,22 +1112,22 @@
     </row>
     <row r="13" spans="1:9" ht="20.25">
       <c r="A13" s="18" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C13" s="12">
         <v>45637</v>
       </c>
       <c r="D13" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="12" t="s">
-        <v>49</v>
-      </c>
       <c r="F13" s="24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G13" s="14"/>
       <c r="H13" s="14" t="s">
@@ -1084,19 +1142,19 @@
         <v>17</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F14" s="23" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G14" s="13"/>
       <c r="H14" s="14" t="s">
@@ -1108,20 +1166,20 @@
     </row>
     <row r="15" spans="1:9" ht="37.5">
       <c r="A15" s="22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B15" s="19"/>
       <c r="C15" s="3" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="4" t="s">
@@ -1133,37 +1191,49 @@
     </row>
     <row r="16" spans="1:9" ht="56.25">
       <c r="A16" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
+        <v>35</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>67</v>
+      </c>
       <c r="F16" s="10" t="s">
         <v>20</v>
       </c>
       <c r="G16" s="4"/>
       <c r="H16" s="4" t="s">
-        <v>15</v>
+        <v>69</v>
       </c>
       <c r="I16" s="4">
-        <v>0</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="56.25">
       <c r="A17" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
+        <v>37</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="F17" s="10" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="G17" s="4"/>
       <c r="H17" s="4" t="s">
@@ -1175,7 +1245,7 @@
     </row>
     <row r="18" spans="1:9" ht="37.5">
       <c r="A18" s="21" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B18" s="11"/>
       <c r="C18" s="12">
@@ -1184,11 +1254,11 @@
       <c r="D18" s="12">
         <v>45334</v>
       </c>
-      <c r="E18" s="12">
-        <v>2</v>
+      <c r="E18" s="12" t="s">
+        <v>46</v>
       </c>
       <c r="F18" s="23" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G18" s="13"/>
       <c r="H18" s="14" t="s">
@@ -1200,22 +1270,22 @@
     </row>
     <row r="19" spans="1:9" ht="20.25">
       <c r="A19" s="16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C19" s="12">
-        <v>45302</v>
+        <v>45303</v>
       </c>
       <c r="D19" s="12">
-        <v>45515</v>
+        <v>45303</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="F19" s="24" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14" t="s">
@@ -1227,22 +1297,22 @@
     </row>
     <row r="20" spans="1:9" ht="20.25">
       <c r="A20" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="12">
+        <v>45334</v>
+      </c>
+      <c r="D20" s="12">
+        <v>45334</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="24" t="s">
         <v>42</v>
-      </c>
-      <c r="B20" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="C20" s="12">
-        <v>45302</v>
-      </c>
-      <c r="D20" s="12">
-        <v>45515</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="F20" s="24" t="s">
-        <v>45</v>
       </c>
       <c r="G20" s="14"/>
       <c r="H20" s="14" t="s">
@@ -1253,7 +1323,17 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4"/>
+  <phoneticPr fontId="5"/>
+  <hyperlinks>
+    <hyperlink ref="G9" r:id="rId1" xr:uid="{8EF108BC-8789-40D1-B048-EE1726145743}"/>
+    <hyperlink ref="G10" r:id="rId2" xr:uid="{9DECE325-DFAB-4311-B61E-6AAB32C35C48}"/>
+    <hyperlink ref="G11" r:id="rId3" xr:uid="{46538F4C-0334-4EB0-808B-13F419636D5C}"/>
+    <hyperlink ref="G3" r:id="rId4" xr:uid="{24BC1503-B55D-48C6-A590-E5B857203E13}"/>
+    <hyperlink ref="G4" r:id="rId5" xr:uid="{91297F02-0DA0-4C5C-A75D-4A4D415897FF}"/>
+    <hyperlink ref="G5" r:id="rId6" xr:uid="{EEEBE184-3EA7-4170-8198-D74AD9C41C4C}"/>
+    <hyperlink ref="G6" r:id="rId7" xr:uid="{DBA500C4-C3A6-41C9-8C32-547A10439F9C}"/>
+    <hyperlink ref="G7" r:id="rId8" xr:uid="{156E5DD5-33D9-402F-B930-C6AC3F236C9B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1517,16 +1597,16 @@
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F9428BE-9C52-42F9-94DD-BCAEB7A63D69}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="86b2c21e-bc8a-47d8-90cc-43181eba94ed"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="81e90ab8-9e7d-4b67-ba12-d147179b0223"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="86b2c21e-bc8a-47d8-90cc-43181eba94ed"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>